<commit_message>
cargando datos y corrigiendo errores
</commit_message>
<xml_diff>
--- a/qr_data.xlsx
+++ b/qr_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,85 +436,282 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>QR_Data</t>
+          <t>Unnamed: 0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Apellido</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Fecha</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Hora</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/lastorres.bags/</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2023-11-12</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>23:55:50</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/lastorres.bags/</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2023-11-12</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>23:55:48</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/lastorres.bags/</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2023-11-12</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>23:55:48</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://www.instagram.com/lastorres.bags/</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2023-11-12</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>23:55:47</t>
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>44189151</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Majolli</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Facundo</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>02:48:43</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>44189151</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Majolli</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Facundo</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>02:55:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>44189151</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Majolli</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Facundo</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>02:57:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>44189151</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Majolli</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Facundo</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>02:58:06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Test de app, funciona correctamente
</commit_message>
<xml_diff>
--- a/qr_data.xlsx
+++ b/qr_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,10 +486,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>44189151</t>
-        </is>
+      <c r="A3" t="n">
+        <v>44189151</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -509,6 +507,83 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>07:57:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>37128854</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bazan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ruth</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>08:01:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>37128854</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bazan</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ruth</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>08:06:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>27775770</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Guiñazu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alejandro</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>08:08:40</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se corrigio errores detectados en test
</commit_message>
<xml_diff>
--- a/qr_data.xlsx
+++ b/qr_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,10 +561,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>27775770</t>
-        </is>
+      <c r="A6" t="n">
+        <v>27775770</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -584,6 +582,58 @@
       <c r="E6" t="inlineStr">
         <is>
           <t>08:08:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>44189151</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Majolli</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Facundo</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>08:26:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>31949304</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Reynoso</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Anahi</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>08:34:09</t>
         </is>
       </c>
     </row>

</xml_diff>